<commit_message>
Fix tagging exercises for Assessments when the same exercise appears as pre- and post- in one row
</commit_message>
<xml_diff>
--- a/spec/fixtures/sample_assessments_tags.xlsx
+++ b/spec/fixtures/sample_assessments_tags.xlsx
@@ -301,13 +301,13 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.75"/>
   </cols>
@@ -388,19 +388,19 @@
         <v>5</v>
       </c>
       <c r="H2" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="J2" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="J2" s="6" t="n">
+      <c r="K2" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="K2" s="7" t="n">
+      <c r="L2" s="7" t="n">
         <v>9</v>
-      </c>
-      <c r="L2" s="7" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3089,7 +3089,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.87"/>
@@ -3128,7 +3128,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="n">

</xml_diff>